<commit_message>
Pat's minor edits to manuscript
</commit_message>
<xml_diff>
--- a/results/tables/tables.xlsx
+++ b/results/tables/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17100" yWindow="3240" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="23220" yWindow="4380" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,18 +325,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -533,46 +527,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,54 +558,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,10 +606,66 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1021,240 +998,243 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="26">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="35" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="3">
         <v>90</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="5">
         <v>114</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="3">
         <v>31</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="5">
         <v>113</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="3">
         <v>121</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="5">
         <v>227</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="36" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6" ht="26">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="39">
         <v>167</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="41">
         <v>144</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="42" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" thickBot="1"/>
-    <row r="12" spans="1:6" ht="61" thickBot="1">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:6" ht="52" customHeight="1" thickBot="1">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="15">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="16">
         <v>241483</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="17">
         <v>181112</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="18">
         <v>229409</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="15">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="16">
         <v>4588174</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="17">
         <v>720343</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="18">
         <v>2619847</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" thickBot="1">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="20">
         <v>0.17699999999999999</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="21">
         <v>14247488</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="22">
         <v>2236856</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="23">
         <v>8135316</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
rerendered with fixed citations
</commit_message>
<xml_diff>
--- a/results/tables/tables.xlsx
+++ b/results/tables/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="6980" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="21900" yWindow="6540" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,6 +324,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -630,6 +636,7 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,7 +661,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -999,31 +1005,32 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A17" sqref="A12:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="39"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="26">
       <c r="A2" s="1"/>
@@ -1186,7 +1193,7 @@
       <c r="E14" s="18">
         <v>221359</v>
       </c>
-      <c r="G14" s="43"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="14" t="s">
@@ -1204,7 +1211,7 @@
       <c r="E15" s="18">
         <v>2188854</v>
       </c>
-      <c r="G15" s="43"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="19" t="s">
@@ -1222,24 +1229,24 @@
       <c r="E16" s="23">
         <v>6723534</v>
       </c>
-      <c r="G16" s="43"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="G18" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1248,8 +1255,9 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A17:E18"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added regular markdown file of manuscript
</commit_message>
<xml_diff>
--- a/results/tables/tables.xlsx
+++ b/results/tables/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21200" yWindow="6080" windowWidth="25600" windowHeight="16300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21200" yWindow="6080" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -50,27 +50,6 @@
     <t>n=198</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>15.7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> (10.6-20.7)</t>
-    </r>
-  </si>
-  <si>
     <t>Any Lesions</t>
   </si>
   <si>
@@ -111,13 +90,15 @@
     <t>True Positives identified by FIT</t>
   </si>
   <si>
+    <t>*Number of persons in the United States in 2010, 50-75 years of age, was 80,494,283.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>75.0</t>
     </r>
@@ -125,8 +106,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (67.5-82.5)</t>
     </r>
@@ -137,8 +117,64 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>91.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (86.7-958)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>15.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (10.6-20.7)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>45.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">  (38.4-52.5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>38.1</t>
     </r>
@@ -146,8 +182,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (32.7-43.4)</t>
     </r>
@@ -158,8 +193,26 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>62.9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (57.2-67.9)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>97.1</t>
     </r>
@@ -167,8 +220,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (94.2-99.4)</t>
     </r>
@@ -179,71 +231,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>45.5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">  (38.4-52.5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>62.9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> (57.2-67.9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>91.7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> (86.7-958)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>90.1</t>
     </r>
@@ -251,14 +239,10 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Cambria"/>
-        <scheme val="major"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (85.5-94.2)</t>
     </r>
-  </si>
-  <si>
-    <t>*Number of persons in the United States in 2010, 50-75 years of age, was 80,494,283.</t>
   </si>
 </sst>
 </file>
@@ -294,26 +278,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -330,6 +294,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -559,118 +540,118 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -1025,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1040,150 +1021,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="40"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="26">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="24" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="32" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="33">
         <v>90</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="35">
         <v>110</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="33">
+        <v>31</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="35">
+        <v>90</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="33">
+        <v>121</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="35">
+        <v>200</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <v>31</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5">
-        <v>90</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="37"/>
+    </row>
+    <row r="7" spans="1:7" ht="26">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
-        <v>121</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5">
-        <v>200</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="1:7" ht="26">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="24" t="s">
+      <c r="D7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="E7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" thickBot="1">
-      <c r="A8" s="29" t="s">
+      <c r="B8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="31">
+      <c r="C8" s="40">
         <v>167</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="33">
+      <c r="D8" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="42">
         <v>155</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>29</v>
+      <c r="F8" s="43" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="G14" s="35"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="G15" s="35"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="G16" s="35"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="35"/>
+      <c r="G18" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1191,7 +1172,7 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1206,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1219,95 +1200,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="37" thickBot="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C3" s="10">
+        <v>241483</v>
+      </c>
+      <c r="D3" s="11">
+        <v>181112</v>
+      </c>
+      <c r="E3" s="12">
+        <v>221359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="B4" s="9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C4" s="10">
+        <v>4588174</v>
+      </c>
+      <c r="D4" s="11">
+        <v>883960</v>
+      </c>
+      <c r="E4" s="12">
+        <v>2188854</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" thickBot="1">
+      <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="C5" s="15">
+        <v>14247488</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1600841</v>
+      </c>
+      <c r="E5" s="17">
+        <v>6723534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="15">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C3" s="16">
-        <v>241483</v>
-      </c>
-      <c r="D3" s="17">
-        <v>181112</v>
-      </c>
-      <c r="E3" s="18">
-        <v>221359</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="15">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="C4" s="16">
-        <v>4588174</v>
-      </c>
-      <c r="D4" s="17">
-        <v>883960</v>
-      </c>
-      <c r="E4" s="18">
-        <v>2188854</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1">
-      <c r="A5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="20">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="C5" s="21">
-        <v>14247488</v>
-      </c>
-      <c r="D5" s="22">
-        <v>1600841</v>
-      </c>
-      <c r="E5" s="23">
-        <v>6723534</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>